<commit_message>
recalculated cmip6 oeks15 periods for new model ensemble
</commit_message>
<xml_diff>
--- a/data/gwl_lists/GWLs_CMIP6_OEKS15_lookup_table.xlsx
+++ b/data/gwl_lists/GWLs_CMIP6_OEKS15_lookup_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbecsi/Desktop/Arbeit/Qgis/data/AAR2/GWLs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2906D12D-E74C-F94C-8AED-83722762B845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA21C422-535A-8943-8AF2-DDB30E79C74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12740" yWindow="500" windowWidth="38400" windowHeight="22120" xr2:uid="{489E0962-2F52-8142-A44B-9CA53DE3A000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22120" xr2:uid="{489E0962-2F52-8142-A44B-9CA53DE3A000}"/>
   </bookViews>
   <sheets>
     <sheet name="lookup_table" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="90">
   <si>
     <t>OEKS15 ensemble member</t>
   </si>
@@ -74,9 +74,6 @@
     <t>SDM_MOHC-HadGEM2-ES_rcp26_r1i1p1_SMHI-RCA4_all</t>
   </si>
   <si>
-    <t>2011-2030</t>
-  </si>
-  <si>
     <t>2044-2063</t>
   </si>
   <si>
@@ -131,15 +128,9 @@
     <t>2022-2041</t>
   </si>
   <si>
-    <t>2042-2061</t>
-  </si>
-  <si>
     <t>SDM_ICHEC-EC-EARTH_rcp45_r1i1p1_KNMI-RACMO22E</t>
   </si>
   <si>
-    <t>2021-2040</t>
-  </si>
-  <si>
     <t>2055-2074</t>
   </si>
   <si>
@@ -149,9 +140,6 @@
     <t>2028-2047</t>
   </si>
   <si>
-    <t>2063-2082</t>
-  </si>
-  <si>
     <t>SDM_IPSL-IPSL-CM5A-MR_rcp45_r1i1p1_IPSL-INERIS-WRF331F</t>
   </si>
   <si>
@@ -173,15 +161,9 @@
     <t>2031-2050</t>
   </si>
   <si>
-    <t>2059-2078</t>
-  </si>
-  <si>
     <t>SDM_MOHC-HadGEM2-ES_rcp45_r1i1p1_SMHI-RCA4</t>
   </si>
   <si>
-    <t>2017-2036</t>
-  </si>
-  <si>
     <t>2033-2052</t>
   </si>
   <si>
@@ -209,18 +191,12 @@
     <t>2056-2075</t>
   </si>
   <si>
-    <t>2073-2092</t>
-  </si>
-  <si>
     <t>SDM_CNRM-CERFACS-CNRM-CM5_rcp85_r1i1p1_SMHI-RCA4</t>
   </si>
   <si>
     <t>2052-2071</t>
   </si>
   <si>
-    <t>2070-2089</t>
-  </si>
-  <si>
     <t>SDM_ICHEC-EC-EARTH_rcp85_r12i1p1_CLMcom-CCLM4-8-17</t>
   </si>
   <si>
@@ -233,21 +209,12 @@
     <t>2018-2037</t>
   </si>
   <si>
-    <t>2030-2049</t>
-  </si>
-  <si>
     <t>2049-2068</t>
   </si>
   <si>
     <t>SDM_ICHEC-EC-EARTH_rcp85_r1i1p1_KNMI-RACMO22E</t>
   </si>
   <si>
-    <t>2020-2039</t>
-  </si>
-  <si>
-    <t>2077-2096</t>
-  </si>
-  <si>
     <t>SDM_ICHEC-EC-EARTH_rcp85_r3i1p1_DMI-HIRHAM5</t>
   </si>
   <si>
@@ -257,33 +224,21 @@
     <t>SDM_IPSL-IPSL-CM5A-MR_rcp85_r1i1p1_IPSL-INERIS-WRF331F</t>
   </si>
   <si>
-    <t>2041-2060</t>
-  </si>
-  <si>
     <t>SDM_IPSL-IPSL-CM5A-MR_rcp85_r1i1p1_SMHI-RCA4</t>
   </si>
   <si>
     <t>2025-2044</t>
   </si>
   <si>
-    <t>2061-2080</t>
-  </si>
-  <si>
     <t>SDM_MOHC-HadGEM2-ES_rcp85_r1i1p1_CLMcom-CCLM4-8-17</t>
   </si>
   <si>
-    <t>2013-2032</t>
-  </si>
-  <si>
     <t>2057-2076</t>
   </si>
   <si>
     <t>SDM_MOHC-HadGEM2-ES_rcp85_r1i1p1_SMHI-RCA4</t>
   </si>
   <si>
-    <t>2012-2031</t>
-  </si>
-  <si>
     <t>SDM_MPI-M-MPI-ESM-LR_rcp85_r1i1p1_CLMcom-CCLM4-8-17</t>
   </si>
   <si>
@@ -296,10 +251,61 @@
     <t>SDM_MPI-M-MPI-ESM-LR_rcp85_r1i1p1_SMHI-RCA4</t>
   </si>
   <si>
-    <t>2058-2077</t>
-  </si>
-  <si>
     <t>2071-2090</t>
+  </si>
+  <si>
+    <t>2023-2042</t>
+  </si>
+  <si>
+    <t>2014-2033</t>
+  </si>
+  <si>
+    <t>2026-2045</t>
+  </si>
+  <si>
+    <t>2010-2029</t>
+  </si>
+  <si>
+    <t>2007-2026</t>
+  </si>
+  <si>
+    <t>2037-2056</t>
+  </si>
+  <si>
+    <t>2069-2088</t>
+  </si>
+  <si>
+    <t>2034-2053</t>
+  </si>
+  <si>
+    <t>2062-2081</t>
+  </si>
+  <si>
+    <t>2006-2025</t>
+  </si>
+  <si>
+    <t>2075-2094</t>
+  </si>
+  <si>
+    <t>2054-2073</t>
+  </si>
+  <si>
+    <t>2038-2057</t>
+  </si>
+  <si>
+    <t>2053-2072</t>
+  </si>
+  <si>
+    <t>2072-2091</t>
+  </si>
+  <si>
+    <t>2076-2095</t>
+  </si>
+  <si>
+    <t>2065-2084</t>
+  </si>
+  <si>
+    <t>2078-2097</t>
   </si>
 </sst>
 </file>
@@ -365,6 +371,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDADADA"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -676,7 +687,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -706,13 +717,16 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -720,402 +734,420 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>79</v>
+      </c>
+      <c r="D18" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="E24" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E25" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="E26" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D28" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>62</v>
+        <v>88</v>
+      </c>
+      <c r="E29" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E31" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D32" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="E32" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B33" t="s">
         <v>81</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="E33" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>62</v>
+        <v>19</v>
+      </c>
+      <c r="E34" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" t="s">
         <v>85</v>
       </c>
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" t="s">
-        <v>86</v>
-      </c>
       <c r="E35" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>